<commit_message>
fazendo a funcionalidade de projeto
</commit_message>
<xml_diff>
--- a/AADSP-DB.xlsx
+++ b/AADSP-DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto" r:id="rId2" sheetId="1" state="visible"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -46,18 +46,42 @@
     <t xml:space="preserve">Prazo de Entrega</t>
   </si>
   <si>
-    <t xml:space="preserve">Projeto A</t>
+    <t xml:space="preserve">Projeto ABC</t>
   </si>
   <si>
     <t xml:space="preserve">01/02/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">Projeto BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/02/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projeto C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projeto D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nível de Importancia</t>
   </si>
   <si>
     <t xml:space="preserve">Vitor vitinho</t>
   </si>
   <si>
+    <t xml:space="preserve">Azinho</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nivel de Experiência</t>
   </si>
   <si>
@@ -79,6 +103,9 @@
     <t xml:space="preserve">Tela Login</t>
   </si>
   <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Título</t>
   </si>
   <si>
@@ -103,6 +130,9 @@
     <t xml:space="preserve">Media</t>
   </si>
   <si>
+    <t xml:space="preserve">Tarefa B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Status</t>
   </si>
   <si>
@@ -148,10 +178,10 @@
     <t xml:space="preserve">Teste de Instalação</t>
   </si>
   <si>
-    <t>Tarefa B</t>
-  </si>
-  <si>
-    <t>Media</t>
+    <t>Projeto CD</t>
+  </si>
+  <si>
+    <t>01/01/202</t>
   </si>
 </sst>
 </file>
@@ -335,7 +365,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -378,6 +408,74 @@
       </c>
       <c r="E2" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>70000</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -415,13 +513,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -429,10 +527,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -443,10 +541,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -468,10 +566,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -487,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -495,9 +593,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -536,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -544,10 +653,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +675,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2"/>
@@ -585,13 +694,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -602,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -611,6 +720,23 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -630,9 +756,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E8" activeCellId="0" pane="topLeft" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -646,22 +772,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -669,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -678,33 +804,33 @@
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -739,28 +865,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -795,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -803,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -844,16 +970,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -888,7 +1014,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Commit Vincular Desenvolvedor De Requisito a Release
</commit_message>
<xml_diff>
--- a/AADSP-DB.xlsx
+++ b/AADSP-DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="8" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto" r:id="rId2" sheetId="1" state="visible"/>
@@ -15,6 +15,8 @@
     <sheet name="Bugs" r:id="rId6" sheetId="5" state="visible"/>
     <sheet name="Sprint" r:id="rId7" sheetId="6" state="visible"/>
     <sheet name="PlanoTeste" r:id="rId8" sheetId="7" state="visible"/>
+    <sheet name="Requisito_Sprint" r:id="rId9" sheetId="8" state="visible"/>
+    <sheet name="Desenvolvedor_Requisito_Sprint" r:id="rId10" sheetId="9" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -115,6 +117,9 @@
     <t xml:space="preserve">Vitor</t>
   </si>
   <si>
+    <t xml:space="preserve">aaa</t>
+  </si>
+  <si>
     <t xml:space="preserve">Título</t>
   </si>
   <si>
@@ -148,16 +153,25 @@
     <t xml:space="preserve">Data Fim</t>
   </si>
   <si>
-    <t xml:space="preserve">1.0.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/02/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15/02/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendente</t>
+    <t xml:space="preserve">VAI TOMAR NO CU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/03/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/04/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalizada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAAAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/02/2002</t>
   </si>
   <si>
     <t xml:space="preserve">Descricao</t>
@@ -205,25 +219,100 @@
     <t xml:space="preserve">Teste de Integridade</t>
   </si>
   <si>
-    <t>PUTA QUE PARIU</t>
-  </si>
-  <si>
-    <t>01/01/2020</t>
-  </si>
-  <si>
-    <t>01/02/2020</t>
+    <t xml:space="preserve">Id Requisito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinculou Desenvolvedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NívelImpactoAlterações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baixo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Requisito_Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id Desenvolvedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porcentagem</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t>projeto d</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
   <si>
     <t>Pendente</t>
   </si>
   <si>
-    <t>VAI TOMAR NO CUUU</t>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>Finalizada</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>rtert</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>vv</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>AAABB</t>
   </si>
   <si>
     <t>11/03/2019</t>
   </si>
   <si>
     <t>15/04/2019</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -450,6 +539,23 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
@@ -679,6 +785,40 @@
         <v>1</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
@@ -712,28 +852,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -752,32 +892,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
@@ -785,42 +925,93 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -833,7 +1024,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -850,13 +1041,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -864,10 +1055,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -878,10 +1069,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -892,10 +1083,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
@@ -906,10 +1097,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -920,10 +1111,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -934,10 +1125,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>3</v>
@@ -948,10 +1139,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>3</v>
@@ -962,10 +1153,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3</v>
@@ -980,4 +1171,467 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="3" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="25.84" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="20.88" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="18.34" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="24.87" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>25.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
desenvolvimento da rede bayesiana
</commit_message>
<xml_diff>
--- a/AADSP-DB.xlsx
+++ b/AADSP-DB.xlsx
@@ -2,24 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
-    <sheet name="Projeto" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="Stakeholder" r:id="rId3" sheetId="2" state="visible"/>
-    <sheet name="Desenvolvedor" r:id="rId4" sheetId="3" state="visible"/>
-    <sheet name="Requisito" r:id="rId5" sheetId="4" state="visible"/>
-    <sheet name="Bugs" r:id="rId6" sheetId="5" state="visible"/>
-    <sheet name="Sprint" r:id="rId7" sheetId="6" state="visible"/>
-    <sheet name="PlanoTeste" r:id="rId8" sheetId="7" state="visible"/>
-    <sheet name="Requisito_Sprint" r:id="rId9" sheetId="8" state="visible"/>
-    <sheet name="Status_Casos_Teste" r:id="rId10" sheetId="9" state="visible"/>
-    <sheet name="Desenvolvedor_Requisito_Sprint" r:id="rId11" sheetId="10" state="visible"/>
+    <sheet name="Projeto" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Stakeholder" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Desenvolvedor" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Requisito" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Bugs" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sprint" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="PlanoTeste" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Requisito_Sprint" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Status_Casos_Teste" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Desenvolvedor_Requisito_Sprint" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="PredicaoTeste" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -145,6 +146,12 @@
     <t xml:space="preserve">Id_Requisito_Sprint</t>
   </si>
   <si>
+    <t xml:space="preserve">bbbb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Médio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nome </t>
   </si>
   <si>
@@ -199,7 +206,7 @@
     <t xml:space="preserve">2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Vai pra puta que pariu</t>
+    <t xml:space="preserve">aaaa</t>
   </si>
   <si>
     <t xml:space="preserve">2015</t>
@@ -268,9 +275,6 @@
     <t xml:space="preserve">false</t>
   </si>
   <si>
-    <t xml:space="preserve">Médio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Id Requisito Sprint</t>
   </si>
   <si>
@@ -286,22 +290,25 @@
     <t xml:space="preserve">Porcentagem</t>
   </si>
   <si>
-    <t>aaaa</t>
-  </si>
-  <si>
-    <t>Baixo</t>
-  </si>
-  <si>
-    <t>bbbb</t>
-  </si>
-  <si>
-    <t>Médio</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2016</t>
+    <t xml:space="preserve">IdSprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IdRequisito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IdProjeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome Requisito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProbabilidadeAlta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProbabilidadeMedia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProbabilidadeBaixa</t>
   </si>
 </sst>
 </file>
@@ -349,14 +356,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -365,47 +372,47 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -417,16 +424,16 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D:D A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -460,7 +467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -477,7 +484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -494,7 +501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -511,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -528,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -546,9 +553,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -563,29 +570,29 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C3" activeCellId="1" pane="topLeft" sqref="2:2 C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="D:D C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="18.34" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="24.87" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -596,7 +603,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -607,7 +614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
@@ -618,7 +625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
@@ -629,7 +636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>3</v>
       </c>
@@ -640,7 +647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -651,7 +658,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
@@ -662,7 +669,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
@@ -673,7 +680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>8</v>
       </c>
@@ -684,7 +691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -695,7 +702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
@@ -707,9 +714,64 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -724,16 +786,16 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="1" pane="topLeft" sqref="2:2 B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D:D B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -755,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -766,7 +828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -778,9 +840,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -795,16 +857,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D:D A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -826,7 +888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -838,9 +900,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -855,19 +917,19 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="2:2 A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D:D A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="13.65" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -901,7 +963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -918,7 +980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -935,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -952,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -969,11 +1031,11 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -986,25 +1048,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="2:2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:D A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="15.0" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="24.73" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="20.7" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="20.01" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="20.98" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="1023" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
-    <col min="1024" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,30 +1086,30 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.0</v>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1062,67 +1124,67 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D:D A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -1130,70 +1192,70 @@
         <v>31</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" t="s">
-        <v>90</v>
+        <v>58</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1208,20 +1270,20 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D:D A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="28.9" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="20.56" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="23.48" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,128 +1291,128 @@
         <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1365,36 +1427,36 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="1" pane="topLeft" sqref="2:2 A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="D:D A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="25.84" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="20.88" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -1405,16 +1467,16 @@
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1429,30 +1491,30 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="1" pane="topLeft" sqref="2:2 A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="D:D A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
implementando funcionalidade de exclusao
</commit_message>
<xml_diff>
--- a/AADSP-DB.xlsx
+++ b/AADSP-DB.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -330,6 +330,27 @@
   </si>
   <si>
     <t>50</t>
+  </si>
+  <si>
+    <t>Vagner Santana</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>bvbb</t>
+  </si>
+  <si>
+    <t>AAAA</t>
   </si>
 </sst>
 </file>
@@ -1000,15 +1021,15 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>3</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -1296,6 +1317,46 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
implementando sistema de exclusao
</commit_message>
<xml_diff>
--- a/AADSP-DB.xlsx
+++ b/AADSP-DB.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>AAAA</t>
+  </si>
+  <si>
+    <t>Sucesso</t>
+  </si>
+  <si>
+    <t>Sprint 09</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Pendente</t>
   </si>
 </sst>
 </file>
@@ -2030,8 +2045,8 @@
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>81</v>
+      <c r="C12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">

</xml_diff>